<commit_message>
Incorporating LM and profile metadata
</commit_message>
<xml_diff>
--- a/PLP_Rubric_Project/Data/Learner_Profile_8_Jan_2025.xlsx
+++ b/PLP_Rubric_Project/Data/Learner_Profile_8_Jan_2025.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">educational</t>
   </si>
   <si>
-    <t xml:space="preserve">news_artice</t>
+    <t xml:space="preserve">news_article</t>
   </si>
   <si>
     <t xml:space="preserve">diy</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">powerpoint</t>
   </si>
   <si>
-    <t xml:space="preserve">textbook_exerpt</t>
+    <t xml:space="preserve">textbook_excerpt</t>
   </si>
   <si>
     <t xml:space="preserve">minimum_time</t>
@@ -344,15 +344,15 @@
   </sheetPr>
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="132.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="132.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.33"/>
   </cols>

</xml_diff>